<commit_message>
[ADD] ADDING AG-GRID UTILITARY
</commit_message>
<xml_diff>
--- a/data/FOOTPRINT_PLANEJAMENTO_ESTRATEGICO.xlsx
+++ b/data/FOOTPRINT_PLANEJAMENTO_ESTRATEGICO.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emerson\Desktop\Analytics\MATERIAIS POR TEMA\STREAMLIT\APP_FOOTPRINT_PLANEJAMENTO_ESTRATEGICO\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -325,8 +330,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,13 +394,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -433,9 +446,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -467,9 +480,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,9 +515,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -676,14 +691,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -771,10 +788,10 @@
         <v>-23.5398946</v>
       </c>
       <c r="N2">
-        <v>-46.7702766</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>-46.770276600000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -812,13 +829,13 @@
         <v>73</v>
       </c>
       <c r="M3">
-        <v>-22.7923877</v>
+        <v>-22.792387699999999</v>
       </c>
       <c r="N3">
-        <v>-43.3019578</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>-43.301957799999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -856,13 +873,13 @@
         <v>74</v>
       </c>
       <c r="M4">
-        <v>-23.5686493</v>
+        <v>-23.568649300000001</v>
       </c>
       <c r="N4">
-        <v>-46.648073</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>-46.648072999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -906,7 +923,7 @@
         <v>-47.4005279</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -943,14 +960,15 @@
       <c r="L6" t="s">
         <v>76</v>
       </c>
-      <c r="M6">
-        <v>0</v>
+      <c r="M6" t="e">
+        <f>-N</f>
+        <v>#NAME?</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -988,13 +1006,13 @@
         <v>77</v>
       </c>
       <c r="M7">
-        <v>-20.464995</v>
+        <v>-20.464994999999998</v>
       </c>
       <c r="N7">
-        <v>-54.6218864</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>-54.621886400000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1032,13 +1050,13 @@
         <v>78</v>
       </c>
       <c r="M8">
-        <v>-22.9441817</v>
+        <v>-22.944181700000001</v>
       </c>
       <c r="N8">
-        <v>-43.1826049</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>-43.182604900000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1079,10 +1097,10 @@
         <v>-8.062722149999999</v>
       </c>
       <c r="N9">
-        <v>-34.89699854629429</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>-34.896998546294292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1120,13 +1138,13 @@
         <v>80</v>
       </c>
       <c r="M10">
-        <v>-8.06571765</v>
+        <v>-8.0657176499999998</v>
       </c>
       <c r="N10">
-        <v>-34.88214888000604</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>-34.882148880006042</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1167,10 +1185,10 @@
         <v>-26.987257</v>
       </c>
       <c r="N11">
-        <v>-48.9506817</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>-48.950681699999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1211,13 +1229,13 @@
         <v>-29.9369497</v>
       </c>
       <c r="N12">
-        <v>-51.169416</v>
+        <v>-51.169415999999998</v>
       </c>
       <c r="O12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1255,16 +1273,16 @@
         <v>83</v>
       </c>
       <c r="M13">
-        <v>-25.43087</v>
+        <v>-25.430869999999999</v>
       </c>
       <c r="N13">
-        <v>-49.2488523</v>
+        <v>-49.248852300000003</v>
       </c>
       <c r="O13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1302,16 +1320,16 @@
         <v>84</v>
       </c>
       <c r="M14">
-        <v>-22.9152122</v>
+        <v>-22.915212199999999</v>
       </c>
       <c r="N14">
-        <v>-47.0641358</v>
+        <v>-47.064135800000003</v>
       </c>
       <c r="O14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1352,13 +1370,13 @@
         <v>-22.0286075</v>
       </c>
       <c r="N15">
-        <v>-47.9058592</v>
+        <v>-47.905859200000002</v>
       </c>
       <c r="O15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1405,7 +1423,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1446,13 +1464,13 @@
         <v>-30.03314005</v>
       </c>
       <c r="N17">
-        <v>-51.22071319142959</v>
+        <v>-51.220713191429589</v>
       </c>
       <c r="O17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1490,7 +1508,7 @@
         <v>88</v>
       </c>
       <c r="M18">
-        <v>-22.8934625</v>
+        <v>-22.893462499999998</v>
       </c>
       <c r="N18">
         <v>-43.1237852</v>
@@ -1499,7 +1517,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1537,16 +1555,16 @@
         <v>89</v>
       </c>
       <c r="M19">
-        <v>-23.7127624</v>
+        <v>-23.712762399999999</v>
       </c>
       <c r="N19">
-        <v>-46.5257773</v>
+        <v>-46.525777300000001</v>
       </c>
       <c r="O19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1584,16 +1602,16 @@
         <v>90</v>
       </c>
       <c r="M20">
-        <v>-28.2711001</v>
+        <v>-28.271100100000002</v>
       </c>
       <c r="N20">
-        <v>-52.4095764</v>
+        <v>-52.409576399999999</v>
       </c>
       <c r="O20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1631,10 +1649,10 @@
         <v>91</v>
       </c>
       <c r="M21">
-        <v>-22.9311916</v>
+        <v>-22.931191599999998</v>
       </c>
       <c r="N21">
-        <v>-47.0423342</v>
+        <v>-47.042334199999999</v>
       </c>
       <c r="O21" t="s">
         <v>101</v>

</xml_diff>